<commit_message>
get authored data and bind chart
</commit_message>
<xml_diff>
--- a/scripts/TI-Dashboard-Template.xlsx
+++ b/scripts/TI-Dashboard-Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohamedkhalid/Projects/TI-Dashboard/TI-Dashboard/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4519AA9C-2A43-7B41-A43B-852FA5BDC064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79FB2E7F-F092-C842-B8CD-5B0683847788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34100" windowHeight="20280" tabRatio="955" firstSheet="2" activeTab="3" xr2:uid="{FF39CD31-D48F-490A-A10C-4AE871D23273}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34100" windowHeight="20280" tabRatio="955" firstSheet="2" activeTab="11" xr2:uid="{FF39CD31-D48F-490A-A10C-4AE871D23273}"/>
   </bookViews>
   <sheets>
     <sheet name="GenAI Startup Overview 2024" sheetId="10" r:id="rId1"/>
@@ -22,9 +22,9 @@
     <sheet name="Tab_NA_5-10years" sheetId="4" r:id="rId7"/>
     <sheet name="Tab_NA_10-15years" sheetId="5" r:id="rId8"/>
     <sheet name="Tab_NA_15+years" sheetId="6" r:id="rId9"/>
-    <sheet name="Tab_IND_5-10years" sheetId="7" r:id="rId10"/>
-    <sheet name="Tab_IND_10-15years" sheetId="8" r:id="rId11"/>
-    <sheet name="Tab_IND_15+years" sheetId="9" r:id="rId12"/>
+    <sheet name="Tab_IN_5-10years" sheetId="7" r:id="rId10"/>
+    <sheet name="Tab_IN_10-15years" sheetId="8" r:id="rId11"/>
+    <sheet name="Tab_IN_15+years" sheetId="9" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1219,6 +1219,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2110,7 +2111,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA4F842-37AC-4C2E-88CD-B381D10211AB}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="87" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="125" workbookViewId="0">
       <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
@@ -3045,8 +3046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13F9CC07-0331-4014-9756-3231C331C16E}">
   <dimension ref="A2:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="A2:E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z37" sqref="Z37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -17815,7 +17816,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView zoomScale="206" zoomScaleNormal="206" workbookViewId="0">
-      <selection activeCell="D21" sqref="A1:XFD1048576"/>
+      <selection activeCell="D7" sqref="D7:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -18058,8 +18059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81C371B4-3FCF-43AA-9CD6-6A16097B3200}">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Created separate files retain, reskill and recruit section
Created separate files retain, reskill and recruit section
Cleaned up map-helper.js
Cleaned up excel-to-json-helper.js
Edited Excel sheet
</commit_message>
<xml_diff>
--- a/scripts/TI-Dashboard-Template.xlsx
+++ b/scripts/TI-Dashboard-Template.xlsx
@@ -8,23 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohamedkhalid/Projects/TI-Dashboard/TI-Dashboard/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79FB2E7F-F092-C842-B8CD-5B0683847788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF275DC8-A084-EA41-9575-573C07CE92F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34100" windowHeight="20280" tabRatio="955" firstSheet="2" activeTab="11" xr2:uid="{FF39CD31-D48F-490A-A10C-4AE871D23273}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34100" windowHeight="20280" tabRatio="955" activeTab="11" xr2:uid="{FF39CD31-D48F-490A-A10C-4AE871D23273}"/>
   </bookViews>
   <sheets>
     <sheet name="GenAI Startup Overview 2024" sheetId="10" r:id="rId1"/>
     <sheet name="Gen AI Emerging skills 2024" sheetId="11" r:id="rId2"/>
     <sheet name="Competitor Insights" sheetId="12" r:id="rId3"/>
-    <sheet name="Tab_EMEA_5-10years" sheetId="1" r:id="rId4"/>
-    <sheet name="Tab_EMEA _10-15years" sheetId="2" r:id="rId5"/>
-    <sheet name="Tab_EMEA_15+years" sheetId="3" r:id="rId6"/>
-    <sheet name="Tab_NA_5-10years" sheetId="4" r:id="rId7"/>
-    <sheet name="Tab_NA_10-15years" sheetId="5" r:id="rId8"/>
-    <sheet name="Tab_NA_15+years" sheetId="6" r:id="rId9"/>
-    <sheet name="Tab_IN_5-10years" sheetId="7" r:id="rId10"/>
-    <sheet name="Tab_IN_10-15years" sheetId="8" r:id="rId11"/>
-    <sheet name="Tab_IN_15+years" sheetId="9" r:id="rId12"/>
+    <sheet name="EMEA 5-10years" sheetId="1" r:id="rId4"/>
+    <sheet name="EMEA 10-15years" sheetId="2" r:id="rId5"/>
+    <sheet name="EMEA 15+years" sheetId="3" r:id="rId6"/>
+    <sheet name="NA 5-10years" sheetId="4" r:id="rId7"/>
+    <sheet name="NA 10-15years" sheetId="5" r:id="rId8"/>
+    <sheet name="NA 15+years" sheetId="6" r:id="rId9"/>
+    <sheet name="IN 5-10years" sheetId="7" r:id="rId10"/>
+    <sheet name="IN 10-15years" sheetId="8" r:id="rId11"/>
+    <sheet name="IN 15+years" sheetId="9" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -17816,7 +17816,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView zoomScale="206" zoomScaleNormal="206" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:H8"/>
+      <selection activeCell="B1" sqref="B1:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Startup overview chart logic
</commit_message>
<xml_diff>
--- a/scripts/TI-Dashboard-Template.xlsx
+++ b/scripts/TI-Dashboard-Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohamedkhalid/Projects/TI-Dashboard/TI-Dashboard/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F848446-59B7-644F-AAB8-2D428A4A3B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5030232-F306-014F-9D1E-14B907768D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20340" tabRatio="955" activeTab="1" xr2:uid="{FF39CD31-D48F-490A-A10C-4AE871D23273}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20260" tabRatio="955" xr2:uid="{FF39CD31-D48F-490A-A10C-4AE871D23273}"/>
   </bookViews>
   <sheets>
     <sheet name="GenAI Startup Overview 2024" sheetId="10" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <sheet name="IN 15+years" sheetId="9" r:id="rId12"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Gen AI Emerging skills 2024'!$D$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Gen AI Emerging skills 2024'!$A$1:$F$410</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1163,9 +1163,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1595,218 +1602,219 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2121,10 +2129,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA4F842-37AC-4C2E-88CD-B381D10211AB}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16"/>
@@ -2142,10 +2150,11 @@
     <col min="11" max="11" width="17.6640625" style="68" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.83203125" style="68" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.5" style="68" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.6640625" style="68"/>
+    <col min="14" max="14" width="10.1640625" style="68" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.6640625" style="68"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" s="67" t="s">
         <v>193</v>
       </c>
@@ -2185,8 +2194,11 @@
       <c r="M1" s="67" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" s="77" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="69" t="s">
         <v>205</v>
       </c>
@@ -2227,7 +2239,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:14">
       <c r="A3" s="69" t="s">
         <v>216</v>
       </c>
@@ -2268,7 +2280,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:14">
       <c r="A4" s="69" t="s">
         <v>224</v>
       </c>
@@ -2309,7 +2321,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:14">
       <c r="A5" s="69" t="s">
         <v>233</v>
       </c>
@@ -2350,7 +2362,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:14">
       <c r="A6" s="69" t="s">
         <v>240</v>
       </c>
@@ -2391,7 +2403,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:14">
       <c r="A7" s="69" t="s">
         <v>248</v>
       </c>
@@ -2432,7 +2444,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:14">
       <c r="A8" s="69" t="s">
         <v>256</v>
       </c>
@@ -2473,7 +2485,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:14">
       <c r="A9" s="69" t="s">
         <v>264</v>
       </c>
@@ -2496,9 +2508,7 @@
         <v>214</v>
       </c>
       <c r="H9" s="72"/>
-      <c r="I9" s="72" t="s">
-        <v>214</v>
-      </c>
+      <c r="I9" s="72"/>
       <c r="J9" s="70" t="s">
         <v>267</v>
       </c>
@@ -2510,7 +2520,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:14">
       <c r="A10" s="69" t="s">
         <v>268</v>
       </c>
@@ -2551,7 +2561,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:14">
       <c r="A11" s="69" t="s">
         <v>275</v>
       </c>
@@ -3244,8 +3254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E10A0AFA-A819-4C4A-9D97-B9DBFF563266}">
   <dimension ref="A1:W410"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E1" sqref="D1:E1"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>